<commit_message>
Trial and Report Updates
Included some information about data trials as well as pictures, some
is also written down and will be added to the report today.
</commit_message>
<xml_diff>
--- a/TemperatureVsRates.xlsx
+++ b/TemperatureVsRates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="180" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="580" windowWidth="25600" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Can we compensate for motor failure through higher extruder temperature without sacrificing print quality</t>
   </si>
@@ -52,6 +52,27 @@
   </si>
   <si>
     <t>At this point the true maximum flow rate based on the current motor is reached, the next step would be to test the x and y axis steppers to see I they can keep up(data sheet can be created after a simple test because need to observe to know if my test will work)</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>Flow rates</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow abs filament, Octave, </t>
   </si>
 </sst>
 </file>
@@ -452,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -469,6 +490,9 @@
       </c>
     </row>
     <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -477,6 +501,9 @@
       </c>
       <c r="D3" t="s">
         <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
       </c>
       <c r="I3" t="s">
         <v>1</v>
@@ -590,253 +617,421 @@
         <v>270</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
-      <c r="B19" s="1" t="s">
+    <row r="16" spans="1:14">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="I19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="2:14">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="2:14">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="2:14">
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1800</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2200</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2400</v>
-      </c>
-      <c r="G22" s="1">
-        <v>2600</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J22" s="1">
-        <v>1800</v>
-      </c>
-      <c r="K22" s="1">
-        <v>2000</v>
-      </c>
-      <c r="L22" s="1">
-        <v>2200</v>
-      </c>
-      <c r="M22" s="1">
-        <v>2400</v>
-      </c>
-      <c r="N22" s="1">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14">
-      <c r="B23" s="1">
-        <v>190</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="I23" s="1">
-        <v>190</v>
-      </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="2:14">
-      <c r="B24" s="1">
-        <f xml:space="preserve"> 5 + B23</f>
-        <v>195</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="I24" s="1">
-        <f xml:space="preserve"> 5 + I23</f>
-        <v>195</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="2:14">
-      <c r="B25" s="1">
-        <f t="shared" ref="B25:B29" si="0" xml:space="preserve"> 5 + B24</f>
-        <v>200</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="I25" s="1">
-        <f t="shared" ref="I25:I29" si="1" xml:space="preserve"> 5 + I24</f>
-        <v>200</v>
-      </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="2:14">
-      <c r="B26" s="1">
-        <f t="shared" si="0"/>
-        <v>205</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="I26" s="1">
-        <f t="shared" si="1"/>
-        <v>205</v>
-      </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="H26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="2:14">
-      <c r="B27" s="1">
-        <f t="shared" si="0"/>
-        <v>210</v>
-      </c>
+    <row r="27" spans="1:14">
+      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="I27" s="1">
-        <f t="shared" si="1"/>
-        <v>210</v>
-      </c>
+      <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="2:14">
-      <c r="B28" s="1">
-        <f t="shared" si="0"/>
-        <v>215</v>
-      </c>
-      <c r="C28" s="1"/>
+    <row r="28" spans="1:14">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="I28" s="1">
-        <f t="shared" si="1"/>
-        <v>215</v>
-      </c>
-      <c r="J28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="2:14">
-      <c r="B29" s="1">
-        <f t="shared" si="0"/>
-        <v>220</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="I29" s="1">
-        <f t="shared" si="1"/>
-        <v>220</v>
-      </c>
+    <row r="29" spans="1:14">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1">
+        <v>748</v>
+      </c>
+      <c r="D29" s="1">
+        <v>831</v>
+      </c>
+      <c r="E29" s="1">
+        <v>914</v>
+      </c>
+      <c r="F29" s="1">
+        <v>997</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1081</v>
+      </c>
+      <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="32" spans="2:14">
-      <c r="B32" t="s">
+    <row r="30" spans="1:14">
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1800</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2200</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2400</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2600</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1800</v>
+      </c>
+      <c r="K30" s="1">
+        <v>2000</v>
+      </c>
+      <c r="L30" s="1">
+        <v>2200</v>
+      </c>
+      <c r="M30" s="1">
+        <v>2400</v>
+      </c>
+      <c r="N30" s="1">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="B31" s="1">
+        <v>190</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="I31" s="1">
+        <v>190</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="B32" s="1">
+        <f xml:space="preserve"> 5 + B31</f>
+        <v>195</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="I32" s="1">
+        <f xml:space="preserve"> 5 + I31</f>
+        <v>195</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="1">
+        <f t="shared" ref="B33:B37" si="0" xml:space="preserve"> 5 + B32</f>
+        <v>200</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="I33" s="1">
+        <f t="shared" ref="I33:I37" si="1" xml:space="preserve"> 5 + I32</f>
+        <v>200</v>
+      </c>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>205</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="I34" s="1">
+        <f t="shared" si="1"/>
+        <v>205</v>
+      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="I35" s="1">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>215</v>
+      </c>
+      <c r="C36" s="1">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="I36" s="1">
+        <f t="shared" si="1"/>
+        <v>215</v>
+      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="C37" s="1">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="I37" s="1">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="1">
+        <v>225</v>
+      </c>
+      <c r="C38" s="1">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39" s="1">
+        <v>230</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" s="1">
+        <v>235</v>
+      </c>
+      <c r="C40" s="1">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="1">
+        <v>240</v>
+      </c>
+      <c r="C41" s="1">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" s="1">
+        <v>245</v>
+      </c>
+      <c r="C42" s="1">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+    </row>
+    <row r="43" spans="2:14">
+      <c r="B43" s="1">
+        <v>250</v>
+      </c>
+      <c r="C43" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
+      <c r="B44" s="1">
+        <v>260</v>
+      </c>
+      <c r="C44" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14">
+      <c r="B45" s="1">
+        <v>260</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14">
+      <c r="B47" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
+    <row r="48" spans="2:14">
+      <c r="B48" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="s">
+    <row r="49" spans="2:3">
+      <c r="B49" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="C55" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>